<commit_message>
update RT PULSE 8 HP TH bom
</commit_message>
<xml_diff>
--- a/RT_Pulse_8_HP_decoder/RT_Pulse_8_HP_TH_BOM_2023-10-03.xlsx
+++ b/RT_Pulse_8_HP_decoder/RT_Pulse_8_HP_TH_BOM_2023-10-03.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="95">
   <si>
     <t xml:space="preserve">No.</t>
   </si>
@@ -447,9 +447,6 @@
   </si>
   <si>
     <t xml:space="preserve">RES-TH_BD2.4-L6.3-P10.30-D0.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.2kΩ</t>
   </si>
   <si>
     <t xml:space="preserve">MFP50SBRE52-2K2</t>
@@ -694,16 +691,17 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="69.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="64.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.94"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1029,13 +1027,13 @@
         <v>76</v>
       </c>
       <c r="E16" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="G16" s="0" t="s">
         <v>78</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1046,70 +1044,70 @@
         <v>7</v>
       </c>
       <c r="C17" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="F17" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="G17" s="0" t="s">
         <v>82</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="F18" s="0" t="s">
         <v>86</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="F19" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>61</v>
       </c>
       <c r="F20" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="G20" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>